<commit_message>
stock groups but for real this time
</commit_message>
<xml_diff>
--- a/tickers.xlsx
+++ b/tickers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benka\Documents\GitHub\rebal-v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77F264F-7D85-4FED-B36C-0965A5C2D3A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B603E92E-D86D-447A-ADA5-E2DBBF27C55C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>AMZN</t>
   </si>
@@ -408,7 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -673,10 +673,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D807BEF-3897-46B4-9E0A-71866A6A0159}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -703,6 +703,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>0.1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
create buckets from excel and optimize each bucket
</commit_message>
<xml_diff>
--- a/tickers.xlsx
+++ b/tickers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benka\Documents\GitHub\rebal-v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B603E92E-D86D-447A-ADA5-E2DBBF27C55C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7875DE73-B456-4D14-BB44-A9DFB207D47A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>AMZN</t>
   </si>
@@ -89,6 +89,18 @@
   </si>
   <si>
     <t>group3</t>
+  </si>
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>Bucket</t>
+  </si>
+  <si>
+    <t>MaxWeight</t>
+  </si>
+  <si>
+    <t>MinWeight</t>
   </si>
 </sst>
 </file>
@@ -406,263 +418,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>0.05</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>0.01</v>
+      </c>
+      <c r="D5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>0.01</v>
+      </c>
+      <c r="D6">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>0.01</v>
+      </c>
+      <c r="D7">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>0.01</v>
+      </c>
+      <c r="D8">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>0.01</v>
+      </c>
+      <c r="D9">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>0.01</v>
+      </c>
+      <c r="D10">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>0.05</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>0.01</v>
+      </c>
+      <c r="D12">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>0.01</v>
+      </c>
+      <c r="D13">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>0.01</v>
+      </c>
+      <c r="D14">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>0.01</v>
+      </c>
+      <c r="D15">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>0.01</v>
+      </c>
+      <c r="D16">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>0.01</v>
+      </c>
+      <c r="D17">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
       </c>
       <c r="C18">
-        <v>5.0000000000000001E-3</v>
+        <v>0.15</v>
       </c>
       <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>0.15</v>
+      </c>
+      <c r="D19">
         <v>1</v>
       </c>
     </row>
@@ -673,28 +697,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D807BEF-3897-46B4-9E0A-71866A6A0159}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>18</v>
-      </c>
-      <c r="B1">
-        <v>0.1</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>19</v>
       </c>
       <c r="B2">
         <v>0.1</v>
@@ -703,14 +725,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>0.1</v>
       </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>0.1</v>
+      </c>
+      <c r="C4">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
each individual security has its own constraints in the excel
reverted back to OG rebal-v2 afte realizing that you can set a constraint for each security. removed the buckets from the excel. should be more streamlined
</commit_message>
<xml_diff>
--- a/tickers.xlsx
+++ b/tickers.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benka\Documents\GitHub\rebal-v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7875DE73-B456-4D14-BB44-A9DFB207D47A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7696F4E8-F6FE-4E42-AA79-62C85453BE8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>AMZN</t>
   </si>
@@ -82,19 +81,7 @@
     <t>SO</t>
   </si>
   <si>
-    <t>group1</t>
-  </si>
-  <si>
-    <t>group2</t>
-  </si>
-  <si>
-    <t>group3</t>
-  </si>
-  <si>
     <t>Ticker</t>
-  </si>
-  <si>
-    <t>Bucket</t>
   </si>
   <si>
     <t>MaxWeight</t>
@@ -418,308 +405,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>0.05</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>0.05</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4">
-        <v>0.05</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>0.01</v>
-      </c>
-      <c r="D5">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6">
-        <v>0.01</v>
-      </c>
-      <c r="D6">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>0.01</v>
-      </c>
-      <c r="D7">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8">
-        <v>0.01</v>
-      </c>
-      <c r="D8">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9">
-        <v>0.01</v>
-      </c>
-      <c r="D9">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10">
-        <v>0.01</v>
-      </c>
-      <c r="D10">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11">
-        <v>0.05</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12">
-        <v>0.01</v>
-      </c>
-      <c r="D12">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13">
-        <v>0.01</v>
-      </c>
-      <c r="D13">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14">
-        <v>0.01</v>
-      </c>
-      <c r="D14">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15">
-        <v>0.01</v>
-      </c>
-      <c r="D15">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16">
-        <v>0.01</v>
-      </c>
-      <c r="D16">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17">
-        <v>0.01</v>
-      </c>
-      <c r="D17">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18">
-        <v>0.15</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19">
-        <v>0.15</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D807BEF-3897-46B4-9E0A-71866A6A0159}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -727,10 +437,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -738,12 +448,177 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.01</v>
+      </c>
+      <c r="C5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.01</v>
+      </c>
+      <c r="C6">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.01</v>
+      </c>
+      <c r="C7">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.01</v>
+      </c>
+      <c r="C8">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.01</v>
+      </c>
+      <c r="C10">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.05</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0.01</v>
+      </c>
+      <c r="C12">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0.01</v>
+      </c>
+      <c r="C13">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0.01</v>
+      </c>
+      <c r="C14">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0.01</v>
+      </c>
+      <c r="C15">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0.01</v>
+      </c>
+      <c r="C16">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0.01</v>
+      </c>
+      <c r="C17">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>0.15</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>0.15</v>
+      </c>
+      <c r="C19">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed from arithmetic returns to log returns
</commit_message>
<xml_diff>
--- a/tickers.xlsx
+++ b/tickers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benka\Documents\GitHub\rebal-v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7696F4E8-F6FE-4E42-AA79-62C85453BE8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F46D0A6-2363-4F93-8D50-DB0393552516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,33 +24,53 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ben Karenas</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{AC37DE21-6476-4AA4-87FF-FF25C0120A30}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sum of column must be less than 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{893F4EA8-EB0D-48B4-85EA-7584DAE5D269}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sum of column must be greater than 1</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>AMZN</t>
   </si>
   <si>
-    <t>ADBE</t>
-  </si>
-  <si>
-    <t>INTC</t>
-  </si>
-  <si>
-    <t>BG</t>
-  </si>
-  <si>
     <t>GLTR</t>
   </si>
   <si>
-    <t>MET</t>
-  </si>
-  <si>
-    <t>NEE</t>
-  </si>
-  <si>
-    <t>IBM</t>
-  </si>
-  <si>
     <t>OHI</t>
   </si>
   <si>
@@ -60,27 +80,15 @@
     <t>AXP</t>
   </si>
   <si>
-    <t>CACI</t>
-  </si>
-  <si>
     <t>CNC</t>
   </si>
   <si>
-    <t>EMR</t>
-  </si>
-  <si>
     <t>LDOS</t>
   </si>
   <si>
     <t>MDT</t>
   </si>
   <si>
-    <t>MPLX</t>
-  </si>
-  <si>
-    <t>SO</t>
-  </si>
-  <si>
     <t>Ticker</t>
   </si>
   <si>
@@ -88,19 +96,95 @@
   </si>
   <si>
     <t>MinWeight</t>
+  </si>
+  <si>
+    <t>FDX</t>
+  </si>
+  <si>
+    <t>WMT</t>
+  </si>
+  <si>
+    <t>CORE</t>
+  </si>
+  <si>
+    <t>BLK</t>
+  </si>
+  <si>
+    <t>LMT</t>
+  </si>
+  <si>
+    <t>ORCL</t>
+  </si>
+  <si>
+    <t>NTRS</t>
+  </si>
+  <si>
+    <t>TSM</t>
+  </si>
+  <si>
+    <t>SJM</t>
+  </si>
+  <si>
+    <t>MDLZ</t>
+  </si>
+  <si>
+    <t>REGI</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>MSFT</t>
+  </si>
+  <si>
+    <t>JNJ</t>
+  </si>
+  <si>
+    <t>TPH</t>
+  </si>
+  <si>
+    <t>NRZ</t>
+  </si>
+  <si>
+    <t>VIRT</t>
+  </si>
+  <si>
+    <t>BX</t>
+  </si>
+  <si>
+    <t>MRK</t>
+  </si>
+  <si>
+    <t>PFE</t>
+  </si>
+  <si>
+    <t>SYY</t>
+  </si>
+  <si>
+    <t>EMB</t>
+  </si>
+  <si>
+    <t>TLT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -404,32 +488,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -437,10 +521,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B3">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -448,10 +532,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -459,76 +543,76 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>0.01</v>
       </c>
       <c r="C5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>0.01</v>
       </c>
       <c r="C6">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>0.01</v>
       </c>
       <c r="C7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>0.01</v>
       </c>
       <c r="C8">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>0.01</v>
       </c>
       <c r="C9">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>0.01</v>
       </c>
       <c r="C10">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B11">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -536,76 +620,76 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>0.01</v>
       </c>
       <c r="C12">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>0.01</v>
       </c>
       <c r="C13">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>0.01</v>
       </c>
       <c r="C14">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>0.01</v>
       </c>
       <c r="C15">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>0.01</v>
       </c>
       <c r="C16">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>0.01</v>
       </c>
       <c r="C17">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B18">
-        <v>0.15</v>
+        <v>0.01</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -613,16 +697,160 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B19">
-        <v>0.15</v>
+        <v>0.01</v>
       </c>
       <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>0.01</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21">
+        <v>0.01</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>0.01</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>0.01</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>0.01</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25">
+        <v>0.01</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>0.01</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>0.01</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>0.01</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <v>0.01</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>0.01</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>0.01</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32">
+        <v>0.01</v>
+      </c>
+      <c r="C32">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add group min/max weights
</commit_message>
<xml_diff>
--- a/tickers.xlsx
+++ b/tickers.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benka\Documents\GitHub\rebal-v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FD7401-536D-414F-91B7-980AE604B7B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8C4798-A1A1-4D60-8260-E1B55E2725FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tickers" sheetId="1" r:id="rId1"/>
+    <sheet name="Groups" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,12 +68,78 @@
         </r>
       </text>
     </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{BFCA52C1-26EF-4F31-BCCA-4553F95BA13C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>All groups must be present on "Groups" tab</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ben Karenas</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{E55C183F-C3D0-4E45-8384-4E2E693273E9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Groups must correspond to a group on the "Tickers" tab</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{720C352D-15A0-4A41-B0FC-9CA3B34E725D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sum of column must be less than 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{BEB5494D-44CC-4143-A4BD-342DF9CCF6C8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sum of column must be greater than 1</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
   <si>
     <t>AMZN</t>
   </si>
@@ -170,17 +237,35 @@
     <t>SYY</t>
   </si>
   <si>
-    <t>EMB</t>
-  </si>
-  <si>
     <t>TLT</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Equity</t>
+  </si>
+  <si>
+    <t>Commod</t>
+  </si>
+  <si>
+    <t>RE</t>
+  </si>
+  <si>
+    <t>Bond</t>
+  </si>
+  <si>
+    <t>GroupMin</t>
+  </si>
+  <si>
+    <t>GroupMax</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +279,20 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -213,16 +312,47 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -532,19 +662,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -554,8 +684,11 @@
       <c r="C1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -565,8 +698,11 @@
       <c r="C2">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -576,8 +712,11 @@
       <c r="C3">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -585,10 +724,13 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C4">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -598,8 +740,12 @@
       <c r="C5">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -609,8 +755,11 @@
       <c r="C6">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -620,8 +769,11 @@
       <c r="C7">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -631,8 +783,11 @@
       <c r="C8">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -642,8 +797,11 @@
       <c r="C9">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -653,8 +811,11 @@
       <c r="C10">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -664,8 +825,11 @@
       <c r="C11">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -675,8 +839,11 @@
       <c r="C12">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -686,8 +853,11 @@
       <c r="C13">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -697,8 +867,11 @@
       <c r="C14">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -708,8 +881,11 @@
       <c r="C15">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -719,8 +895,11 @@
       <c r="C16">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -730,187 +909,309 @@
       <c r="C17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C18">
+        <v>0.05</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C19">
+        <v>0.05</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C20">
+        <v>0.05</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C21">
+        <v>0.05</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C22">
+        <v>0.05</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C23">
+        <v>0.05</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C24">
+        <v>0.05</v>
+      </c>
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C25">
+        <v>0.05</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C26">
+        <v>0.05</v>
+      </c>
+      <c r="D26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C27">
+        <v>0.05</v>
+      </c>
+      <c r="D27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="B18">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C18">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C19">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C20">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C21">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C22">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C23">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C24">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C25">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C26">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="B28">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
         <v>2</v>
       </c>
-      <c r="B27">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C27">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C28">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
       <c r="B29">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C29">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>1</v>
       </c>
       <c r="B30">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C30">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="B31">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C31">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32">
-        <v>0.2</v>
-      </c>
-      <c r="C32">
-        <v>0.4</v>
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>SUM(C:C)&lt;1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>SUM(C:C)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>SUM(B:B)&gt;1</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>SUM(B:B)&lt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD9FF80-EA65-4692-B28E-535A5E3B7E02}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <v>0.02</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C5">
+        <v>0.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>SUM(B:B)&gt;1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>SUM(B:B)&lt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>SUM(C:C)&lt;1</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>SUM(B:B)&lt;1</formula>
+      <formula>SUM(C:C)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added calculations for ann return, vol, and utility
</commit_message>
<xml_diff>
--- a/tickers.xlsx
+++ b/tickers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benka\Documents\GitHub\rebal-v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8C4798-A1A1-4D60-8260-E1B55E2725FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622E12F6-6D57-4E36-A79E-7AE60BDBF396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>All groups must be present on "Groups" tab</t>
         </r>
@@ -100,7 +100,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Groups must correspond to a group on the "Tickers" tab</t>
         </r>
@@ -139,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
   <si>
     <t>AMZN</t>
   </si>
@@ -259,13 +259,25 @@
   </si>
   <si>
     <t>GroupMax</t>
+  </si>
+  <si>
+    <t>IAU</t>
+  </si>
+  <si>
+    <t>SLV</t>
+  </si>
+  <si>
+    <t>PALL</t>
+  </si>
+  <si>
+    <t>PPLT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,13 +298,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -662,19 +667,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.84375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -688,7 +691,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -702,7 +705,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -716,7 +719,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -730,7 +733,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -745,7 +748,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -759,7 +762,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -773,7 +776,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -787,7 +790,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -801,7 +804,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -815,7 +818,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -829,7 +832,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -843,7 +846,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -857,7 +860,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -871,7 +874,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -885,7 +888,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -899,7 +902,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -913,7 +916,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -927,7 +930,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -941,7 +944,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -955,7 +958,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -969,7 +972,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -983,7 +986,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1011,7 +1014,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1025,7 +1028,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1039,7 +1042,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1053,7 +1056,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1067,7 +1070,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -1081,7 +1084,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1095,17 +1098,73 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>32</v>
       </c>
-      <c r="B31">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C31">
+      <c r="B35">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C35">
         <v>1</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D35" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1137,12 +1196,12 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1153,7 +1212,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1164,7 +1223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1175,7 +1234,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1186,7 +1245,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1194,7 +1253,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C5">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>